<commit_message>
Implemented and removed all necessary files
</commit_message>
<xml_diff>
--- a/fwf-carturesti-internship-practice-dispatcher/Data/Config.xlsx
+++ b/fwf-carturesti-internship-practice-dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-carturesti-internship-practice-dispatcher\fwf-carturesti-internship-practice-dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81E94A4-18EF-4BD6-9B53-C0688CE50666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60598AB6-E8AA-444F-BA4C-8D702109814F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -95,98 +95,208 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>BooksLimit</t>
+  </si>
+  <si>
+    <t>BestPickBooks</t>
+  </si>
+  <si>
+    <t>InputMailAddress</t>
+  </si>
+  <si>
+    <t>InputMailAddresses</t>
+  </si>
+  <si>
+    <t>PriceLimit</t>
+  </si>
+  <si>
+    <t>fwf-carturesti-internship-practice-dispatcher</t>
+  </si>
+  <si>
+    <t>BestPickBooksQueue</t>
+  </si>
+  <si>
+    <t>CarturestiURL</t>
+  </si>
+  <si>
+    <t>https://www.carturesti.ro/</t>
+  </si>
+  <si>
+    <t>https://www.emag.ro/</t>
+  </si>
+  <si>
+    <t>eMAGURL</t>
+  </si>
+  <si>
+    <t>Carturesti_SortBy</t>
+  </si>
+  <si>
+    <t>Carturesti_BooksPerPage</t>
+  </si>
+  <si>
+    <t>Preț (ascendent)</t>
+  </si>
+  <si>
+    <t>This is the option to sort the books on the page.</t>
+  </si>
+  <si>
+    <t>The quantity of books per page.</t>
+  </si>
+  <si>
+    <t>These will be the columns to build the DT for Carturesti books.</t>
+  </si>
+  <si>
+    <t>CarturestiDT_Columns</t>
+  </si>
+  <si>
+    <t>Carturesti_Sheet</t>
+  </si>
+  <si>
+    <t>Carturesti</t>
+  </si>
+  <si>
+    <t>Name of sheet in Output report for Carturesti books.</t>
+  </si>
+  <si>
+    <t>Book price is higher than the threshold that's been set.</t>
+  </si>
+  <si>
+    <t>If a book has a higher price that the given threshold, will throw this BE.</t>
+  </si>
+  <si>
+    <t>NOTE: Change this acording to your machine.</t>
+  </si>
+  <si>
+    <t>eMAG</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>eMAGDT_Columns</t>
+  </si>
+  <si>
+    <t>These will be the columns to build the DT for eMAG books.</t>
+  </si>
+  <si>
+    <t>Name of sheet in Output report for eMAG books.</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\OutputReport.xlsx</t>
+  </si>
+  <si>
+    <t>OutputReportPath</t>
+  </si>
+  <si>
+    <t>eMAG_Sheet</t>
+  </si>
+  <si>
+    <t>eMAG_BooksPerPage</t>
+  </si>
+  <si>
+    <t>60 pe pagina</t>
+  </si>
+  <si>
+    <t>Pret crescator</t>
+  </si>
+  <si>
+    <t>eMAG_SortBy</t>
+  </si>
+  <si>
+    <t>BE1_Message</t>
+  </si>
+  <si>
+    <t>Title,Author,Price</t>
+  </si>
+  <si>
+    <t>Book details that will be written in BE sheet in Output Report.</t>
+  </si>
+  <si>
+    <t>BE_Sheet</t>
+  </si>
+  <si>
+    <t>BE_DT_Columns</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>BooksLimit</t>
-  </si>
-  <si>
-    <t>BestPickBooks</t>
-  </si>
-  <si>
-    <t>InputMailAddress</t>
-  </si>
-  <si>
-    <t>InputMailAddresses</t>
-  </si>
-  <si>
-    <t>PriceLimit</t>
-  </si>
-  <si>
-    <t>fwf-carturesti-internship-practice-dispatcher</t>
-  </si>
-  <si>
-    <t>BestPickBooksQueue</t>
-  </si>
-  <si>
-    <t>CarturestiURL</t>
-  </si>
-  <si>
-    <t>https://www.carturesti.ro/</t>
-  </si>
-  <si>
-    <t>https://www.emag.ro/</t>
-  </si>
-  <si>
-    <t>eMAGURL</t>
+  </si>
+  <si>
+    <t>Title,Author,Price,Language,No Pages</t>
+  </si>
+  <si>
+    <t>Title,Author,Overall review, No Reviews,Price</t>
+  </si>
+  <si>
+    <t>ApplicationProcessName</t>
+  </si>
+  <si>
+    <t>chrome.exe</t>
+  </si>
+  <si>
+    <t>If the app cannot be closed gently, the robot will try to kill the process.</t>
+  </si>
+  <si>
+    <t>DelayForFilters</t>
+  </si>
+  <si>
+    <t>This delay will be applied before every activity that selects filters.</t>
   </si>
 </sst>
 </file>
@@ -564,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -612,10 +722,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -623,13 +733,13 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -638,7 +748,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -648,43 +758,174 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1716,18 +1957,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1751,7 +1992,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1773,7 +2014,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1784,7 +2025,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1795,53 +2036,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2845,7 +3086,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2875,35 +3116,35 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>